<commit_message>
Importar cursos en admin
</commit_message>
<xml_diff>
--- a/api/Libro1.xlsx
+++ b/api/Libro1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Codigo</t>
   </si>
@@ -54,25 +54,28 @@
     <t>Periodo</t>
   </si>
   <si>
-    <t>M123B</t>
-  </si>
-  <si>
-    <t>Matematica basica</t>
-  </si>
-  <si>
-    <t>primer semestre</t>
-  </si>
-  <si>
-    <t>Kevin</t>
+    <t>C123M</t>
+  </si>
+  <si>
+    <t>Calculo Monovariable</t>
+  </si>
+  <si>
+    <t>2024-1</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>kevin@gmail.com</t>
+  </si>
+  <si>
+    <t>Andres</t>
   </si>
   <si>
     <t>Orozco</t>
-  </si>
-  <si>
-    <t>kevin@gmail.com</t>
-  </si>
-  <si>
-    <t>Andres</t>
   </si>
   <si>
     <t>andres@gmail.com</t>
@@ -742,7 +745,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -750,12 +753,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
@@ -1297,7 +1294,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
@@ -1369,10 +1366,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -1382,13 +1379,13 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1398,13 +1395,13 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1414,31 +1411,31 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="4">
+      <c r="A8" s="1">
         <v>1005</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Importar cursos validaciones basicas y listado de profesores
</commit_message>
<xml_diff>
--- a/api/Libro1.xlsx
+++ b/api/Libro1.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milog\OneDrive\Desktop\tareas\Univalle\proyecto integrador\Componentes de react TeamEval\nuevo team eval\Team-Eval\api\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4C2DEB-FB97-4F06-B2F0-D6076D5E9FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-105" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,6 +25,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,12 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Codigo</t>
   </si>
   <si>
-    <t>Identificacion</t>
+    <t>Documento</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -91,7 +87,7 @@
     <t>laura@gmail.com</t>
   </si>
   <si>
-    <t>Oscar</t>
+    <t>Alejandro</t>
   </si>
   <si>
     <t>Lopez</t>
@@ -122,13 +118,22 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Fin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +146,7 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -148,6 +154,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,19 +162,341 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -177,215 +506,355 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Coma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Salida" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="19" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Énfasis1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Énfasis1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Énfasis1" xfId="28" builtinId="32"/>
+    <cellStyle name="Énfasis2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="40" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Énfasis5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Énfasis5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Énfasis5" xfId="44" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Énfasis6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <b val="1"/>
         <color theme="1"/>
       </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -396,7 +865,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -424,108 +893,154 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -536,10 +1051,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="D7D7D7"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="101313"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -783,26 +1298,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="21.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="18.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="27.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -936,36 +1451,48 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>1006</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F9" s="1"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11" s="4"/>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="E13" s="4"/>
+    <row r="11" spans="5:5">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="13" spans="5:5">
+      <c r="E13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E5" r:id="rId3" tooltip="mailto:laura@gmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E6" r:id="rId4" tooltip="mailto:oscar@gmail.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E7" r:id="rId5" tooltip="mailto:mario@gmail.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{95CFE23B-ABBE-400C-83AF-6568D9A587D3}"/>
+    <hyperlink ref="E3" r:id="rId1" display="kevin@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId2" display="andres@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId3" display="laura@gmail.com" tooltip="mailto:laura@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId4" display="oscar@gmail.com" tooltip="mailto:oscar@gmail.com"/>
+    <hyperlink ref="E7" r:id="rId5" display="mario@gmail.com" tooltip="mailto:mario@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId6" display="esteban@gmail.com"/>
+    <hyperlink ref="E9" r:id="rId6" display="esteban@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>